<commit_message>
Atualizando a pasta 10
</commit_message>
<xml_diff>
--- a/Atividade versão 10/Diagrama_UML - Versão 1.xlsx
+++ b/Atividade versão 10/Diagrama_UML - Versão 1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20397"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20393"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fatec\Downloads\OneDrive_2023-05-05\Atividade versão 10\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fatec\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8E52E53-3387-448D-8FDC-FDCDD50666AC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05B04E4F-521E-4906-B136-BACBDF78FF18}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{83F40B39-AF77-49D9-ABD3-E7F4F43BB617}"/>
   </bookViews>
@@ -19,6 +19,17 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -97,15 +108,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
@@ -484,7 +492,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>imprimirTodasInformcoes() </a:t>
+            <a:t>mostrarInformacoesDoComputador() </a:t>
           </a:r>
           <a:endParaRPr lang="pt-BR" sz="1200">
             <a:effectLst/>
@@ -639,13 +647,13 @@
       <xdr:col>1</xdr:col>
       <xdr:colOff>190498</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:rowOff>85726</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>428625</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -660,8 +668,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="800098" y="714375"/>
-          <a:ext cx="5114927" cy="3400425"/>
+          <a:off x="800098" y="714376"/>
+          <a:ext cx="5114927" cy="2438399"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -797,6 +805,21 @@
           </a:r>
         </a:p>
         <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>pegarComputadoresDaInformatica() : ArrayList&lt;Computador&gt;</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
           <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
             <a:lnSpc>
               <a:spcPct val="100000"/>
@@ -824,68 +847,6 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>pegarComputador(String id)  :  Computador</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPts val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPts val="0"/>
-            </a:spcAft>
-            <a:buClrTx/>
-            <a:buSzTx/>
-            <a:buFontTx/>
-            <a:buNone/>
-            <a:tabLst/>
-            <a:defRPr/>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="pt-BR" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>pegarTodosComputadores() : ArrayList&lt;Computador&gt;</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPts val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPts val="0"/>
-            </a:spcAft>
-            <a:buClrTx/>
-            <a:buSzTx/>
-            <a:buFontTx/>
-            <a:buNone/>
-            <a:tabLst/>
-            <a:defRPr/>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="pt-BR" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
             <a:t>alugarComputador</a:t>
           </a:r>
           <a:r>
@@ -1039,120 +1000,8 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>imprimirSolicitacoesComputador()</a:t>
-          </a:r>
-          <a:endParaRPr lang="pt-BR" sz="1100" baseline="0">
-            <a:solidFill>
-              <a:schemeClr val="lt1"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:latin typeface="+mn-lt"/>
-            <a:ea typeface="+mn-ea"/>
-            <a:cs typeface="+mn-cs"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="pt-BR" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>imprimirSolicitacoesManutencao()</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPts val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPts val="0"/>
-            </a:spcAft>
-            <a:buClrTx/>
-            <a:buSzTx/>
-            <a:buFontTx/>
-            <a:buNone/>
-            <a:tabLst/>
-            <a:defRPr/>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="pt-BR" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>contarComputadores()  :  int</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="pt-BR" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>contarSolicitacoesComputador</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="pt-BR"/>
-            <a:t>()  :  int</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="pt-BR" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>contarSolicitacoesManutencao</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="pt-BR"/>
-            <a:t>()  :  int</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="pt-BR" sz="1100">
-            <a:solidFill>
-              <a:schemeClr val="lt1"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:latin typeface="+mn-lt"/>
-            <a:ea typeface="+mn-ea"/>
-            <a:cs typeface="+mn-cs"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="pt-BR" sz="1100">
-            <a:solidFill>
-              <a:schemeClr val="lt1"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:latin typeface="+mn-lt"/>
-            <a:ea typeface="+mn-ea"/>
-            <a:cs typeface="+mn-cs"/>
-          </a:endParaRPr>
+            <a:t>contarEstoque()  :  int</a:t>
+          </a:r>
         </a:p>
         <a:p>
           <a:endParaRPr lang="pt-BR" sz="1100">
@@ -1429,7 +1278,7 @@
           <a:pPr algn="l"/>
           <a:r>
             <a:rPr lang="pt-BR" sz="1200"/>
-            <a:t>pegarComputador (String id)  :  Computador</a:t>
+            <a:t>pegarComputadorDoEstoque (String id)  :  Computador</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -1440,14 +1289,14 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>428625</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>52388</xdr:rowOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>47626</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
       <xdr:colOff>333374</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>109538</xdr:rowOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>52388</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1464,9 +1313,9 @@
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="5915025" y="2147888"/>
-          <a:ext cx="6000749" cy="266700"/>
+        <a:xfrm>
+          <a:off x="5915025" y="1933576"/>
+          <a:ext cx="6000749" cy="214312"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
@@ -1497,15 +1346,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>309562</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>190499</xdr:rowOff>
+      <xdr:colOff>309561</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>571499</xdr:colOff>
+      <xdr:colOff>571498</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>100012</xdr:rowOff>
+      <xdr:rowOff>100013</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1523,8 +1372,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="16200000" flipH="1">
-          <a:off x="4391024" y="3081337"/>
-          <a:ext cx="1243013" cy="3309937"/>
+          <a:off x="3910011" y="2600325"/>
+          <a:ext cx="2205038" cy="3309937"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector2">
           <a:avLst/>
@@ -1908,8 +1757,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4CFBEE9-8D85-4DD3-A9B7-5D0074A72ED7}">
   <dimension ref="B1:AC25"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="Z28" sqref="Z28"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1921,15 +1770,15 @@
   <sheetData>
     <row r="1" spans="2:29" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:29" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J2" s="4" t="s">
+      <c r="J2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4"/>
-      <c r="O2" s="4"/>
-      <c r="P2" s="4"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
     </row>
     <row r="3" spans="2:29" ht="17.100000000000001" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="2:29" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -1977,20 +1826,18 @@
     <row r="16" spans="2:29" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="R16" s="2"/>
     </row>
-    <row r="17" spans="10:22" x14ac:dyDescent="0.25">
-      <c r="Q17" s="3"/>
+    <row r="19" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="E19" s="2"/>
     </row>
-    <row r="18" spans="10:22" x14ac:dyDescent="0.25">
-      <c r="J18" s="3"/>
+    <row r="21" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B21" s="2"/>
+      <c r="H21" s="2"/>
     </row>
-    <row r="19" spans="10:22" x14ac:dyDescent="0.25">
-      <c r="J19" s="3"/>
-    </row>
-    <row r="23" spans="10:22" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:22" x14ac:dyDescent="0.25">
       <c r="V23" s="2"/>
     </row>
-    <row r="25" spans="10:22" x14ac:dyDescent="0.25">
-      <c r="Q25" s="3"/>
+    <row r="25" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="D25" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>